<commit_message>
Primer commit en el nuevo repositorio
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataCMS/Login.xlsx
+++ b/src/test/resources/testdataCMS/Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT_FRAMEWORK\AutomationFrameworkSelenium\src\test\resources\testdataCMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Curso\BuildingFramework\AutomationFrameworkSeleniumNotif\src\test\resources\testdataCMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA8CCE8-8C6E-49C1-AAD3-FC5802B361F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F10A761-3177-436C-8343-6A6941320C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3220" yWindow="3290" windowWidth="14400" windowHeight="7370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>function</t>
   </si>
   <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -53,6 +50,18 @@
   </si>
   <si>
     <t>admin@example.com</t>
+  </si>
+  <si>
+    <t>loginFailWithUserPasswordNull</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Redlink123</t>
+  </si>
+  <si>
+    <t>JORUIZ</t>
   </si>
 </sst>
 </file>
@@ -66,7 +75,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -74,13 +83,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -88,7 +98,7 @@
       <u/>
       <sz val="14"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -123,7 +133,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,17 +407,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="18.5"/>
   <cols>
-    <col min="1" max="1" width="37.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -416,70 +426,81 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>123456</v>
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>123456</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>123</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>123456</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>123456</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="J11" s="3"/>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="J12" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>